<commit_message>
add: lapor.py functionality, add: db_manager.py
</commit_message>
<xml_diff>
--- a/db/db_file.xlsx
+++ b/db/db_file.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="reports" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +530,222 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>8f27cb897948b306e14d6b9aa620abd4b0f4474ea8398d3469793c1ca1c5ddaf</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>admin@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Admin Ganteng</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-11-27 20:41:02</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>maddd</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>8f27cb897948b306e14d6b9aa620abd4b0f4474ea8398d3469793c1ca1c5ddaf</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>madd1024@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ahmad hidayat</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2024-12-02 01:06:16</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>report_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>journal_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>journal_url</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>reason</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>is_anonymous</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>reporter_username</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>created_at</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>updated_at</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>RPT001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Educenter</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://jurnal.arkainstitute.co.id/index.php/educenter/index</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>tampilan jurnal terlalu bagus wkwkw</t>
+        </is>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-12-02 01:10:34</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2024-12-02 01:10:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>RPT002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Hexatech</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://jurnal.arkainstitute.co.id/hexatech</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>jurnal sangat bagus hehe</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>maddhdyt</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-12-02 12:16:59</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2024-12-02 12:16:59</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
nambah fitur tracking jurnal yang sudah dilapor
</commit_message>
<xml_diff>
--- a/db/db_file.xlsx
+++ b/db/db_file.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,6 +589,38 @@
         </is>
       </c>
       <c r="F5" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>abcd</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>8d969eef6ecad3c29a3a629280e686cf0c3f5d5a86aff3ca12020c923adc6c92</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>abcd@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>abcd</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2024-12-06 14:00:43</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>user</t>
         </is>
@@ -668,17 +700,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Educenter</t>
+          <t>abc</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://jurnal.arkainstitute.co.id/index.php/educenter/index</t>
+          <t>https://abc.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>tampilan jurnal terlalu bagus wkwkw</t>
+          <t>mencurigakan</t>
         </is>
       </c>
       <c r="E2" t="b">
@@ -692,12 +724,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2024-12-02 01:10:34</t>
+          <t>2024-12-07 20:11:31</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2024-12-02 01:10:34</t>
+          <t>2024-12-07 20:11:31</t>
         </is>
       </c>
     </row>
@@ -709,17 +741,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hexatech</t>
+          <t>jurnalbuaya</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://jurnal.arkainstitute.co.id/hexatech</t>
+          <t>www.buaya.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>jurnal sangat bagus hehe</t>
+          <t>buaya</t>
         </is>
       </c>
       <c r="E3" t="b">
@@ -727,7 +759,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>maddhdyt</t>
+          <t>abcd</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -737,12 +769,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2024-12-02 12:16:59</t>
+          <t>2024-12-07 21:42:20</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2024-12-02 12:16:59</t>
+          <t>2024-12-07 21:42:20</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add: validasi.py fix: report.py and check.py
</commit_message>
<xml_diff>
--- a/db/db_file.xlsx
+++ b/db/db_file.xlsx
@@ -719,7 +719,7 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -729,7 +729,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2024-12-07 20:11:31</t>
+          <t>2024-12-16 12:44:56</t>
         </is>
       </c>
     </row>

</xml_diff>